<commit_message>
filling in the ms
</commit_message>
<xml_diff>
--- a/2018-03-30_pc_trait_data.xlsx
+++ b/2018-03-30_pc_trait_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewnguyen/Desktop/latitudinal_variation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4B46FE6A-BDD1-904E-80F2-E71B9341EF2C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{EF403F75-73DF-A346-8F05-754496E6F2F7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11580" yWindow="5460" windowWidth="37040" windowHeight="19560" xr2:uid="{FB01168B-F473-3344-962C-704E728ED92A}"/>
+    <workbookView xWindow="54780" yWindow="920" windowWidth="37040" windowHeight="19560" xr2:uid="{FB01168B-F473-3344-962C-704E728ED92A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,16 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>PC1</t>
-  </si>
-  <si>
-    <t>PC2</t>
-  </si>
-  <si>
-    <t>PC3</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
   <si>
     <t>Desiccation hardiness</t>
   </si>
@@ -49,13 +40,211 @@
   </si>
   <si>
     <t>Growth Rate</t>
+  </si>
+  <si>
+    <t>bio1</t>
+  </si>
+  <si>
+    <t>bio2</t>
+  </si>
+  <si>
+    <t>bio3</t>
+  </si>
+  <si>
+    <t>bio4</t>
+  </si>
+  <si>
+    <t>bio5</t>
+  </si>
+  <si>
+    <t>bio6</t>
+  </si>
+  <si>
+    <t>bio7</t>
+  </si>
+  <si>
+    <t>bio8</t>
+  </si>
+  <si>
+    <t>bio9</t>
+  </si>
+  <si>
+    <t>bio10</t>
+  </si>
+  <si>
+    <t>bio11</t>
+  </si>
+  <si>
+    <t>bio12</t>
+  </si>
+  <si>
+    <t>bio13</t>
+  </si>
+  <si>
+    <t>bio14</t>
+  </si>
+  <si>
+    <t>bio15</t>
+  </si>
+  <si>
+    <t>bio16</t>
+  </si>
+  <si>
+    <t>bio17</t>
+  </si>
+  <si>
+    <t>bio18</t>
+  </si>
+  <si>
+    <t>bio19</t>
+  </si>
+  <si>
+    <t>PC1 (70%)</t>
+  </si>
+  <si>
+    <t>PC2 (17.5%)</t>
+  </si>
+  <si>
+    <t>PC3 (7.2%)</t>
+  </si>
+  <si>
+    <t>PC1 (47.9%)</t>
+  </si>
+  <si>
+    <t>PC2 (22.3%)</t>
+  </si>
+  <si>
+    <t>PC3 (15.2%)</t>
+  </si>
+  <si>
+    <t>BIO1 = Annual Mean Temperature</t>
+  </si>
+  <si>
+    <t>BIO2 = Mean Diurnal Range (Mean of monthly (max temp - min temp))</t>
+  </si>
+  <si>
+    <t>BIO3 = Isothermality (BIO2/BIO7) (* 100)</t>
+  </si>
+  <si>
+    <t>BIO4 = Temperature Seasonality (standard deviation *100)</t>
+  </si>
+  <si>
+    <t>BIO5 = Max Temperature of Warmest Month</t>
+  </si>
+  <si>
+    <t>BIO6 = Min Temperature of Coldest Month</t>
+  </si>
+  <si>
+    <t>BIO7 = Temperature Annual Range (BIO5-BIO6)</t>
+  </si>
+  <si>
+    <t>BIO8 = Mean Temperature of Wettest Quarter</t>
+  </si>
+  <si>
+    <t>BIO9 = Mean Temperature of Driest Quarter</t>
+  </si>
+  <si>
+    <t>BIO10 = Mean Temperature of Warmest Quarter</t>
+  </si>
+  <si>
+    <t>BIO11 = Mean Temperature of Coldest Quarter</t>
+  </si>
+  <si>
+    <t>BIO12 = Annual Precipitation</t>
+  </si>
+  <si>
+    <t>BIO13 = Precipitation of Wettest Month</t>
+  </si>
+  <si>
+    <t>BIO14 = Precipitation of Driest Month</t>
+  </si>
+  <si>
+    <t>BIO15 = Precipitation Seasonality (Coefficient of Variation)</t>
+  </si>
+  <si>
+    <t>BIO16 = Precipitation of Wettest Quarter</t>
+  </si>
+  <si>
+    <t>BIO17 = Precipitation of Driest Quarter</t>
+  </si>
+  <si>
+    <t>BIO18 = Precipitation of Warmest Quarter</t>
+  </si>
+  <si>
+    <t>BIO19 = Precipitation of Coldest Quarter</t>
+  </si>
+  <si>
+    <t>Call:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lm(formula = Comp.1 ~ Comp.1.1 + Comp.2.1 + I(Comp.2.1^2) + I(Comp.3^2), </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    data = full.dat3)</t>
+  </si>
+  <si>
+    <t>Residuals:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Min       1Q   Median       3Q      Max </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.92676 -0.47154  0.01648  0.38782  0.92392 </t>
+  </si>
+  <si>
+    <t>Coefficients:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              Estimate Std. Error t value Pr(&gt;|t|)    </t>
+  </si>
+  <si>
+    <t>(Intercept)    3.46963    0.42432   8.177 4.17e-07 ***</t>
+  </si>
+  <si>
+    <t>Comp.1.1       0.67059    0.09884   6.784 4.39e-06 ***</t>
+  </si>
+  <si>
+    <t>Comp.2.1      -0.49418    0.09574  -5.162 9.46e-05 ***</t>
+  </si>
+  <si>
+    <t>I(Comp.2.1^2) -0.35483    0.06158  -5.763 2.91e-05 ***</t>
+  </si>
+  <si>
+    <t>I(Comp.3^2)   -1.79143    0.19127  -9.366 6.78e-08 ***</t>
+  </si>
+  <si>
+    <t>---</t>
+  </si>
+  <si>
+    <t>Signif. codes:  0 ‘***’ 0.001 ‘**’ 0.01 ‘*’ 0.05 ‘.’ 0.1 ‘ ’ 1</t>
+  </si>
+  <si>
+    <t>Residual standard error: 0.6316 on 16 degrees of freedom</t>
+  </si>
+  <si>
+    <t>Multiple R-squared:  0.8668,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adjusted R-squared:  0.8334 </t>
+  </si>
+  <si>
+    <t>F-statistic: 26.02 on 4 and 16 DF,  p-value: 7.885e-07</t>
+  </si>
+  <si>
+    <t>Seasonal and Extreme - averagePrecipitation</t>
+  </si>
+  <si>
+    <t>Variable-Average climate</t>
+  </si>
+  <si>
+    <t>Overall precipitation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -63,13 +252,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="22"/>
+      <color rgb="FF3B3B3B"/>
+      <name val="Georgia"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -84,9 +292,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -401,99 +619,495 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9DD21B0-75FB-5842-9CBF-315EC99854C6}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:W21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D6"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="10.83203125" style="1"/>
+    <col min="7" max="7" width="34.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="52.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="48.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" ht="28" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>-0.490037</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.34317209999999998</v>
+      </c>
+      <c r="D2" s="2">
+        <v>-0.27962239999999999</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="4">
+        <v>0.26516800000000001</v>
+      </c>
+      <c r="H2" s="4">
+        <v>-0.10896774200000001</v>
+      </c>
+      <c r="I2" s="4">
+        <v>-0.1285164</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" ht="28" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="B3" s="2">
+        <v>-0.53739499999999996</v>
+      </c>
+      <c r="C3" s="2">
+        <v>-0.135153</v>
+      </c>
+      <c r="D3" s="2">
+        <v>-0.52863289999999996</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="4">
+        <v>-0.25722669999999997</v>
+      </c>
+      <c r="H3" s="4">
+        <v>-7.6654555999999999E-2</v>
+      </c>
+      <c r="I3" s="4">
+        <v>0.22633710000000001</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" ht="28" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="B4" s="2">
+        <v>-0.37535390000000002</v>
+      </c>
+      <c r="C4" s="2">
+        <v>-0.4530245</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.6526035</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="4">
+        <v>0.1501073</v>
+      </c>
+      <c r="H4" s="5">
+        <v>-0.42157630299999999</v>
+      </c>
+      <c r="I4" s="4">
+        <v>-0.17686631999999999</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" ht="28" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2">
+        <v>-0.22749430000000001</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.78707020000000005</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.44275619999999999</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="4">
+        <v>-0.25064340000000002</v>
+      </c>
+      <c r="H5" s="4">
+        <v>0.190235818</v>
+      </c>
+      <c r="I5" s="4">
+        <v>0.14075512000000001</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="28" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1">
-        <v>-0.490037</v>
-      </c>
-      <c r="C2" s="1">
-        <v>0.34317209999999998</v>
-      </c>
-      <c r="D2" s="1">
-        <v>-0.27962239999999999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1">
-        <v>-0.53739499999999996</v>
-      </c>
-      <c r="C3" s="1">
-        <v>-0.135153</v>
-      </c>
-      <c r="D3" s="1">
-        <v>-0.52863289999999996</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1">
-        <v>-0.37535390000000002</v>
-      </c>
-      <c r="C4" s="1">
-        <v>-0.4530245</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0.6526035</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1">
-        <v>-0.22749430000000001</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0.78707020000000005</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0.44275619999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="1">
+      <c r="B6" s="2">
         <v>0.52766100000000005</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="2">
         <v>0.198131</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="2">
         <v>-0.1429484</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="4">
+        <v>0.20550370000000001</v>
+      </c>
+      <c r="H6" s="4">
+        <v>0.26997632700000002</v>
+      </c>
+      <c r="I6" s="4">
+        <v>-9.423774E-2</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" ht="28" x14ac:dyDescent="0.3">
+      <c r="F7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="4">
+        <v>0.26382729999999999</v>
+      </c>
+      <c r="H7" s="4">
+        <v>-0.10364951999999999</v>
+      </c>
+      <c r="I7" s="4">
+        <v>-0.16226789</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" ht="28" x14ac:dyDescent="0.3">
+      <c r="F8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="4">
+        <v>-0.25638559999999999</v>
+      </c>
+      <c r="H8" s="4">
+        <v>0.15732737299999999</v>
+      </c>
+      <c r="I8" s="4">
+        <v>0.16288080999999999</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" ht="28" x14ac:dyDescent="0.3">
+      <c r="F9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="4">
+        <v>0.219664</v>
+      </c>
+      <c r="H9" s="4">
+        <v>7.1865120000000005E-2</v>
+      </c>
+      <c r="I9" s="4">
+        <v>-7.0377380000000003E-2</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" ht="28" x14ac:dyDescent="0.3">
+      <c r="F10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="4">
+        <v>0.26488410000000001</v>
+      </c>
+      <c r="H10" s="4">
+        <v>-0.112811093</v>
+      </c>
+      <c r="I10" s="4">
+        <v>-0.11637652</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="V10" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" ht="28" x14ac:dyDescent="0.3">
+      <c r="F11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="4">
+        <v>0.25557920000000001</v>
+      </c>
+      <c r="H11" s="4">
+        <v>9.1810012999999996E-2</v>
+      </c>
+      <c r="I11" s="4">
+        <v>-0.13764237000000001</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="V11" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" ht="28" x14ac:dyDescent="0.3">
+      <c r="F12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="4">
+        <v>0.26129089999999999</v>
+      </c>
+      <c r="H12" s="4">
+        <v>-0.13535870999999999</v>
+      </c>
+      <c r="I12" s="4">
+        <v>-0.14081539000000001</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="V12" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" ht="28" x14ac:dyDescent="0.3">
+      <c r="F13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="4">
+        <v>0.25767699999999999</v>
+      </c>
+      <c r="H13" s="4">
+        <v>-8.1280239999999993E-3</v>
+      </c>
+      <c r="I13" s="4">
+        <v>0.25485164999999999</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="V13" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" ht="28" x14ac:dyDescent="0.3">
+      <c r="F14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" s="4">
+        <v>0.20240949999999999</v>
+      </c>
+      <c r="H14" s="4">
+        <v>-0.26374516100000001</v>
+      </c>
+      <c r="I14" s="4">
+        <v>0.37966921999999997</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="V14" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" ht="28" x14ac:dyDescent="0.3">
+      <c r="F15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" s="4">
+        <v>0.1902623</v>
+      </c>
+      <c r="H15" s="5">
+        <v>0.38161582599999999</v>
+      </c>
+      <c r="I15" s="4">
+        <v>3.9115629999999998E-2</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="V15" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" ht="28" x14ac:dyDescent="0.3">
+      <c r="F16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G16" s="4">
+        <v>-0.19217899999999999</v>
+      </c>
+      <c r="H16" s="5">
+        <v>-0.330421405</v>
+      </c>
+      <c r="I16" s="4">
+        <v>0.13730606000000001</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="V16" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="6:23" ht="28" x14ac:dyDescent="0.3">
+      <c r="F17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" s="4">
+        <v>0.2290693</v>
+      </c>
+      <c r="H17" s="4">
+        <v>-0.21779625799999999</v>
+      </c>
+      <c r="I17" s="4">
+        <v>0.32147291</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="V17" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="6:23" ht="28" x14ac:dyDescent="0.3">
+      <c r="F18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" s="4">
+        <v>0.19251199999999999</v>
+      </c>
+      <c r="H18" s="5">
+        <v>0.37608965599999999</v>
+      </c>
+      <c r="I18" s="4">
+        <v>8.1862950000000004E-2</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="6:23" ht="28" x14ac:dyDescent="0.3">
+      <c r="F19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G19" s="4">
+        <v>0.18946209999999999</v>
+      </c>
+      <c r="H19" s="4">
+        <v>-5.2124744000000001E-2</v>
+      </c>
+      <c r="I19" s="4">
+        <v>0.60620624000000001</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="V19" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="6:23" ht="28" x14ac:dyDescent="0.3">
+      <c r="F20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G20" s="4">
+        <v>0.20653640000000001</v>
+      </c>
+      <c r="H20" s="5">
+        <v>0.31508312999999999</v>
+      </c>
+      <c r="I20" s="4">
+        <v>0.23480899999999999</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="V20" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="W20" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="6:23" x14ac:dyDescent="0.3">
+      <c r="G21" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="V21" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updating pca trait excel file
</commit_message>
<xml_diff>
--- a/2018-03-30_pc_trait_data.xlsx
+++ b/2018-03-30_pc_trait_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewnguyen/Desktop/latitudinal_variation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{EF403F75-73DF-A346-8F05-754496E6F2F7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{810A5CD4-9FE4-394B-9199-1E82B5562C16}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="54780" yWindow="920" windowWidth="37040" windowHeight="19560" xr2:uid="{FB01168B-F473-3344-962C-704E728ED92A}"/>
+    <workbookView xWindow="51200" yWindow="-260" windowWidth="38400" windowHeight="19600" xr2:uid="{FB01168B-F473-3344-962C-704E728ED92A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -622,7 +622,7 @@
   <dimension ref="A1:W21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="K2" sqref="K2:K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
@@ -706,7 +706,7 @@
       <c r="F3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="5">
         <v>-0.25722669999999997</v>
       </c>
       <c r="H3" s="4">
@@ -767,7 +767,7 @@
       <c r="F5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="5">
         <v>-0.25064340000000002</v>
       </c>
       <c r="H5" s="4">
@@ -839,7 +839,7 @@
       <c r="F8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="5">
         <v>-0.25638559999999999</v>
       </c>
       <c r="H8" s="4">
@@ -962,7 +962,7 @@
       <c r="H14" s="4">
         <v>-0.26374516100000001</v>
       </c>
-      <c r="I14" s="4">
+      <c r="I14" s="5">
         <v>0.37966921999999997</v>
       </c>
       <c r="K14" s="3" t="s">
@@ -996,7 +996,7 @@
       <c r="F16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G16" s="4">
+      <c r="G16" s="5">
         <v>-0.19217899999999999</v>
       </c>
       <c r="H16" s="5">
@@ -1022,7 +1022,7 @@
       <c r="H17" s="4">
         <v>-0.21779625799999999</v>
       </c>
-      <c r="I17" s="4">
+      <c r="I17" s="5">
         <v>0.32147291</v>
       </c>
       <c r="K17" s="3" t="s">
@@ -1059,7 +1059,7 @@
       <c r="H19" s="4">
         <v>-5.2124744000000001E-2</v>
       </c>
-      <c r="I19" s="4">
+      <c r="I19" s="5">
         <v>0.60620624000000001</v>
       </c>
       <c r="K19" s="3" t="s">

</xml_diff>